<commit_message>
iteration to match latest WhizniumSBE standard
</commit_message>
<xml_diff>
--- a/_mdl/IexWznmBui_msdc.xlsx
+++ b/_mdl/IexWznmBui_msdc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpsitech/doc/msdc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF61087-EA86-2A43-AD46-F7CBA57F1078}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7EAAF4-6EBF-F34C-BC46-B96E4F21F2E3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="680" windowWidth="20000" windowHeight="20300" xr2:uid="{5848B4E3-51D9-E54C-8A3A-4EFDBE0EE488}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>ImeIMModule.sref</t>
   </si>
@@ -169,24 +169,34 @@
   </si>
   <si>
     <t>PreMsdcRefDat</t>
+  </si>
+  <si>
+    <t>IexWznmBui v0.9.0</t>
+  </si>
+  <si>
+    <t>ImeIMModule.end</t>
+  </si>
+  <si>
+    <t>ImeIMPreset.end</t>
+  </si>
+  <si>
+    <t>ImeIJMModule.end</t>
+  </si>
+  <si>
+    <t>ImeIMCard.end</t>
+  </si>
+  <si>
+    <t>ImeIJMCardTitle.end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,6 +207,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,11 +243,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -543,293 +568,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065762DA-C4E3-5A45-B8D8-869B5CD41899}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:6" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D12" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="2" t="s">
+    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="3" t="s">
+    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="3" t="s">
+    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    <row r="16" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="B17" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
+    <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
+    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
+    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
+    <row r="22" spans="1:6" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="B22" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F23" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="3" t="s">
+    <row r="24" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="2" t="s">
+    <row r="25" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="3" t="s">
+    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="3" t="s">
+    <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="3" t="s">
+    <row r="28" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
+    <row r="30" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+    <row r="31" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+    <row r="32" spans="1:6" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="B32" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A33" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D34" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F34" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="35" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D35" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E35" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E36" s="2" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>